<commit_message>
mis le total des points dans le excel
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2235899\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2235899\Documents\GitHub\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9701337F-82F4-46F5-9EE2-75E6AEF08B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBBE78A-DFF3-412F-BFCD-6566736F66F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>Code</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>Fait?</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Jad</t>
+  </si>
+  <si>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>Manbir</t>
   </si>
 </sst>
 </file>
@@ -650,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +674,7 @@
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -679,212 +691,287 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4">
+        <f>SUM(C2:C13)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5">
+        <f>SUM(C14:C25)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6">
+        <f>SUM(C26:C36)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7">
+        <f>SUM(C37:C47)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8">
+        <f>SUM(J4:J7)</f>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5">
-        <v>5</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
-        <v>2</v>
-      </c>
-      <c r="C9" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5">
-        <v>5</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5">
-        <v>2</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5">
-        <v>3</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
       <c r="C16" s="4">
         <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="7">
         <v>2</v>
       </c>
       <c r="C17" s="7">
-        <v>5</v>
-      </c>
-      <c r="D17" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="7">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7">
-        <v>3</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B19" s="7">
         <v>1</v>
@@ -892,344 +979,420 @@
       <c r="C19" s="7">
         <v>4</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="4">
         <v>5</v>
       </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="9">
+        <v>2</v>
+      </c>
+      <c r="C22" s="9">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5">
+        <v>2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>4</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="5">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5">
+        <v>3</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
+        <v>2</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="7">
-        <v>1</v>
-      </c>
-      <c r="C23" s="7">
-        <v>2</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="7">
-        <v>1</v>
-      </c>
-      <c r="C24" s="7">
-        <v>3</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="7">
-        <v>1</v>
-      </c>
-      <c r="C25" s="7">
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7">
+        <v>3</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2</v>
+      </c>
+      <c r="C32" s="7">
+        <v>5</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9">
+        <v>2</v>
+      </c>
+      <c r="C33" s="9">
         <v>4</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="4">
-        <v>3</v>
-      </c>
-      <c r="C26" s="4">
+      <c r="D33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+      <c r="C34" s="9">
+        <v>3</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="4">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="7">
-        <v>2</v>
-      </c>
-      <c r="C29" s="7">
-        <v>5</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="7">
-        <v>1</v>
-      </c>
-      <c r="C30" s="7">
-        <v>3</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="9">
-        <v>2</v>
-      </c>
-      <c r="C31" s="9">
-        <v>4</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="4">
-        <v>2</v>
-      </c>
-      <c r="C33" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="4">
-        <v>2</v>
-      </c>
-      <c r="C34" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="9">
-        <v>2</v>
-      </c>
-      <c r="C35" s="9">
-        <v>5</v>
-      </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="D35" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B36" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" s="9">
-        <v>5</v>
-      </c>
-      <c r="D36" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="9">
-        <v>1</v>
-      </c>
-      <c r="C37" s="9">
-        <v>3</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+      <c r="A37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B38" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" s="4">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="4">
-        <v>2</v>
-      </c>
-      <c r="C39" s="4">
-        <v>4</v>
-      </c>
+      <c r="A39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="5">
+        <v>2</v>
+      </c>
+      <c r="C39" s="5">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B40" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" s="4">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="7">
+        <v>2</v>
+      </c>
+      <c r="C41" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="9">
-        <v>1</v>
-      </c>
-      <c r="C41" s="9">
-        <v>2</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="9">
-        <v>1</v>
-      </c>
-      <c r="C42" s="9">
-        <v>2</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+      <c r="A42" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="7">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="8"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="9">
-        <v>2</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
+      <c r="A43" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B44" s="4">
         <v>2</v>
       </c>
       <c r="C44" s="4">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4">
-        <v>2</v>
-      </c>
+      <c r="A45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="9">
+        <v>3</v>
+      </c>
+      <c r="C45" s="9">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B46" s="4">
         <v>2</v>
       </c>
       <c r="C46" s="4">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="4">
+        <v>3</v>
+      </c>
+      <c r="C47" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="9">
-        <v>2</v>
-      </c>
-      <c r="C47" s="9">
-        <v>3</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
+      <c r="D47" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E47">
+    <sortCondition ref="D2:D47"/>
+  </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E47" xr:uid="{39B55DCA-DF27-4E0D-AFDA-2FB583B68122}">
       <formula1>"oui, non"</formula1>

</xml_diff>

<commit_message>
Fait la tâche C2
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2235899\Documents\GitHub\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBBE78A-DFF3-412F-BFCD-6566736F66F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B361A6CF-C3F5-43FE-A373-B50B4B918410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Manbir</t>
+  </si>
+  <si>
+    <t>oui</t>
   </si>
 </sst>
 </file>
@@ -664,17 +667,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="1"/>
+    <col min="1" max="3" width="8.81640625" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -691,7 +694,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -705,7 +708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -719,7 +722,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -741,7 +744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -762,7 +765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -784,7 +787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -805,7 +808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -823,7 +826,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
@@ -838,7 +841,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -852,7 +855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
@@ -867,7 +870,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -882,7 +885,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
@@ -897,7 +900,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -911,7 +914,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -926,7 +929,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
@@ -940,7 +943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
@@ -955,7 +958,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -969,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -984,7 +987,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1027,7 +1030,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +1087,7 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -1099,7 +1102,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1114,7 +1117,7 @@
       </c>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1157,7 +1160,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
@@ -1172,7 +1175,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -1187,7 +1190,7 @@
       </c>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>38</v>
       </c>
@@ -1202,7 +1205,7 @@
       </c>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>48</v>
       </c>
@@ -1231,7 +1234,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1244,8 +1247,11 @@
       <c r="D37" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1274,7 +1280,7 @@
       </c>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1303,7 +1309,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1318,7 +1324,7 @@
       </c>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1332,7 +1338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>37</v>
       </c>
@@ -1361,7 +1367,7 @@
       </c>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Fait la tâche C7
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B361A6CF-C3F5-43FE-A373-B50B4B918410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3D0FC8-A2FA-4F7A-B1F1-61B655D685F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -668,7 +668,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1263,6 +1263,9 @@
       </c>
       <c r="D38" t="s">
         <v>53</v>
+      </c>
+      <c r="E38" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fait la tâche C10
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3D0FC8-A2FA-4F7A-B1F1-61B655D685F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56311B28-640A-4339-A3CF-022F31FEC61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1281,7 +1281,9 @@
       <c r="D39" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">

</xml_diff>

<commit_message>
Fait la tâche C1
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2235899\Documents\GitHub\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AznGa\Documents\GitHub\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBBE78A-DFF3-412F-BFCD-6566736F66F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD62C09-0B89-47F8-95D1-C2AC9B4CBC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="28680" yWindow="-8070" windowWidth="29040" windowHeight="15720" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Manbir</t>
+  </si>
+  <si>
+    <t>oui</t>
   </si>
 </sst>
 </file>
@@ -346,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -665,10 +668,10 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.85546875" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
@@ -909,6 +912,9 @@
       </c>
       <c r="D14" t="s">
         <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
C4: Fixer erreur taxi monte, tache terminer
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56311B28-640A-4339-A3CF-022F31FEC61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2BE07C-C7C1-4997-8E4E-0F1896885241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -667,11 +667,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.81640625" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
@@ -1085,7 +1085,9 @@
       <c r="D26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">

</xml_diff>

<commit_message>
M7, changer logo terminer
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2BE07C-C7C1-4997-8E4E-0F1896885241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF694BF7-C3EE-400B-91C9-313D274392DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1117,7 +1117,9 @@
       <c r="D28" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
@@ -1145,6 +1147,9 @@
       </c>
       <c r="D30" s="6" t="s">
         <v>54</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fait la tâche M9
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56311B28-640A-4339-A3CF-022F31FEC61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7A6696-A30A-474F-B254-C79682C74EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -668,7 +668,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1327,7 +1327,9 @@
       <c r="D42" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">

</xml_diff>

<commit_message>
Fait la tâche M14 Mis les noms des fichiers dans GameSettings
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2235899\Documents\GitHub\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7A6696-A30A-474F-B254-C79682C74EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C67A61-414C-4CC9-BCCE-9069A3D9058D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -668,16 +668,16 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.81640625" style="1"/>
+    <col min="1" max="3" width="8.85546875" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +694,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -722,7 +722,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -744,7 +744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -765,7 +765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -787,7 +787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -808,7 +808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -826,7 +826,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -855,7 +855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -914,7 +914,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -929,7 +929,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
@@ -943,7 +943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
@@ -958,7 +958,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -972,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>38</v>
       </c>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>48</v>
       </c>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1344,8 +1344,11 @@
       <c r="D43" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>37</v>
       </c>
@@ -1374,7 +1377,7 @@
       </c>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1388,7 +1391,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Fin de la tâche M11
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AznGa\Documents\GitHub\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF694BF7-C3EE-400B-91C9-313D274392DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5094053F-680D-40E3-88D1-DB9098635146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>Code</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>Manbir</t>
-  </si>
-  <si>
-    <t>oui</t>
   </si>
 </sst>
 </file>
@@ -239,7 +236,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,19 +251,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.89999084444715716"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,16 +310,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -331,6 +331,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,17 +671,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.81640625" style="1"/>
+    <col min="1" max="3" width="8.85546875" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,48 +698,50 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="10">
+        <v>3</v>
+      </c>
+      <c r="C2" s="10">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10">
+        <v>3</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="11"/>
       <c r="I4" t="s">
         <v>52</v>
       </c>
@@ -744,19 +750,20 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
+        <v>2</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="E5" s="11"/>
       <c r="I5" t="s">
         <v>51</v>
       </c>
@@ -765,20 +772,20 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="11"/>
       <c r="I6" t="s">
         <v>54</v>
       </c>
@@ -787,19 +794,20 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="E7" s="11"/>
       <c r="I7" t="s">
         <v>53</v>
       </c>
@@ -808,440 +816,446 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="E8" s="11"/>
       <c r="J8">
         <f>SUM(J4:J7)</f>
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10">
+        <v>3</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="4">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="10">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="9">
-        <v>1</v>
-      </c>
-      <c r="C12" s="9">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="9">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B13" s="10">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="4">
-        <v>2</v>
-      </c>
-      <c r="C16" s="4">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B16" s="6">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B17" s="6">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="7">
-        <v>1</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="4">
-        <v>3</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="B20" s="6">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6">
         <v>5</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="9">
-        <v>2</v>
-      </c>
-      <c r="C22" s="9">
+      <c r="B22" s="6">
+        <v>2</v>
+      </c>
+      <c r="C22" s="6">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="4">
-        <v>2</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="4">
-        <v>2</v>
-      </c>
-      <c r="C24" s="4">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B24" s="6">
+        <v>2</v>
+      </c>
+      <c r="C24" s="6">
+        <v>3</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="5">
-        <v>2</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B26" s="8">
+        <v>2</v>
+      </c>
+      <c r="C26" s="8">
         <v>4</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="5">
-        <v>3</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="B27" s="8">
+        <v>3</v>
+      </c>
+      <c r="C27" s="8">
         <v>5</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
-      <c r="C28" s="5">
-        <v>3</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8">
+        <v>3</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4">
-        <v>2</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8">
+        <v>2</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="4">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4">
-        <v>2</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="B30" s="8">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
+        <v>2</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="7">
-        <v>1</v>
-      </c>
-      <c r="C31" s="7">
-        <v>3</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8">
+        <v>3</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="7" t="s">
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="7">
-        <v>2</v>
-      </c>
-      <c r="C32" s="7">
+      <c r="B32" s="8">
+        <v>2</v>
+      </c>
+      <c r="C32" s="8">
         <v>5</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="9">
-        <v>2</v>
-      </c>
-      <c r="C33" s="9">
+      <c r="B33" s="8">
+        <v>2</v>
+      </c>
+      <c r="C33" s="8">
         <v>4</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="9">
-        <v>1</v>
-      </c>
-      <c r="C34" s="9">
-        <v>3</v>
-      </c>
-      <c r="D34" s="6" t="s">
+      <c r="B34" s="8">
+        <v>1</v>
+      </c>
+      <c r="C34" s="8">
+        <v>3</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="4">
-        <v>2</v>
-      </c>
-      <c r="C35" s="4">
+      <c r="B35" s="8">
+        <v>2</v>
+      </c>
+      <c r="C35" s="8">
         <v>5</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="9" t="s">
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="9">
-        <v>2</v>
-      </c>
-      <c r="C36" s="9">
-        <v>3</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="B36" s="8">
+        <v>2</v>
+      </c>
+      <c r="C36" s="8">
+        <v>3</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1251,14 +1265,12 @@
       <c r="C37" s="4">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1268,31 +1280,27 @@
       <c r="C38" s="4">
         <v>2</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="5">
-        <v>2</v>
-      </c>
-      <c r="C39" s="5">
+      <c r="B39" s="4">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4">
         <v>5</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -1302,41 +1310,42 @@
       <c r="C40" s="4">
         <v>3</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="7" t="s">
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="7">
-        <v>2</v>
-      </c>
-      <c r="C41" s="7">
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="7" t="s">
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="7">
-        <v>1</v>
-      </c>
-      <c r="C42" s="7">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4">
+        <v>2</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1346,11 +1355,12 @@
       <c r="C43" s="4">
         <v>3</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -1360,26 +1370,27 @@
       <c r="C44" s="4">
         <v>4</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="9" t="s">
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="9">
-        <v>3</v>
-      </c>
-      <c r="C45" s="9">
+      <c r="B45" s="4">
+        <v>3</v>
+      </c>
+      <c r="C45" s="4">
         <v>5</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1389,11 +1400,12 @@
       <c r="C46" s="4">
         <v>4</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>
@@ -1403,9 +1415,10 @@
       <c r="C47" s="4">
         <v>5</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="5" t="s">
         <v>53</v>
       </c>
+      <c r="E47" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E47">

</xml_diff>

<commit_message>
changer icon, train au decolle, effet fondu
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF694BF7-C3EE-400B-91C9-313D274392DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A59AA5C-04D0-4CF9-B721-BF61A6307797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -668,16 +668,16 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.81640625" style="1"/>
+    <col min="1" max="3" width="8.77734375" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +694,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -722,7 +722,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -744,7 +744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -765,7 +765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -787,7 +787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -808,7 +808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -826,7 +826,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -855,7 +855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -914,7 +914,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -929,7 +929,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
@@ -943,7 +943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
@@ -958,7 +958,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -972,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -1195,9 +1195,11 @@
       <c r="D33" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E33" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>38</v>
       </c>
@@ -1212,7 +1214,7 @@
       </c>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1226,7 +1228,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>48</v>
       </c>
@@ -1241,7 +1243,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1258,7 +1260,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1277,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1292,7 +1294,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -1306,7 +1308,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1321,7 +1323,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1336,7 +1338,7 @@
       </c>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1350,7 +1352,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -1364,7 +1366,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>37</v>
       </c>
@@ -1379,7 +1381,7 @@
       </c>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1393,7 +1395,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
4-5 taches presque terminees
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\users\jaldi\Desktop\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF694BF7-C3EE-400B-91C9-313D274392DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8117D8CC-DCBA-4AA5-8731-99130043A2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -721,6 +721,9 @@
       <c r="D3" t="s">
         <v>52</v>
       </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
@@ -735,7 +738,9 @@
       <c r="D4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" t="s">
         <v>52</v>
       </c>
@@ -757,6 +762,9 @@
       <c r="D5" t="s">
         <v>52</v>
       </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
       <c r="I5" t="s">
         <v>51</v>
       </c>
@@ -778,7 +786,9 @@
       <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="I6" t="s">
         <v>54</v>
       </c>
@@ -800,6 +810,9 @@
       <c r="D7" t="s">
         <v>52</v>
       </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
       <c r="I7" t="s">
         <v>53</v>
       </c>
@@ -820,6 +833,9 @@
       </c>
       <c r="D8" t="s">
         <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
       </c>
       <c r="J8">
         <f>SUM(J4:J7)</f>

</xml_diff>

<commit_message>
Fait la tâche M2
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2235899\Documents\GitHub\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C67A61-414C-4CC9-BCCE-9069A3D9058D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA8FDA3-9C58-4984-9852-B19336226B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t>Code</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>oui</t>
+  </si>
+  <si>
+    <t>non</t>
   </si>
 </sst>
 </file>
@@ -667,17 +670,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="1"/>
+    <col min="1" max="3" width="8.81640625" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +697,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +711,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -722,7 +725,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -744,7 +747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -765,7 +768,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -787,7 +790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -808,7 +811,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -826,7 +829,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
@@ -841,7 +844,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -855,7 +858,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
@@ -870,7 +873,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -885,7 +888,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
@@ -900,7 +903,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -914,7 +917,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -929,7 +932,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
@@ -943,7 +946,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
@@ -958,7 +961,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -972,7 +975,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -987,7 +990,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1030,7 +1033,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1087,7 +1090,7 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -1102,7 +1105,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1120,7 @@
       </c>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1160,7 +1163,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
@@ -1175,7 +1178,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -1190,7 +1193,7 @@
       </c>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>38</v>
       </c>
@@ -1205,7 +1208,7 @@
       </c>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>48</v>
       </c>
@@ -1234,7 +1237,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -1298,8 +1301,11 @@
       <c r="D40" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1314,7 +1320,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1328,10 +1334,10 @@
         <v>53</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1348,7 +1354,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>37</v>
       </c>
@@ -1377,7 +1383,7 @@
       </c>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
fais tache A16 + C4 fixé
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA786A8-4A76-4E1E-A90E-DD80C69BA34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F57C41-C5C6-4C81-B1CC-D48978585BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -667,17 +667,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.81640625" style="1"/>
+    <col min="1" max="3" width="8.77734375" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +694,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -722,7 +722,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -744,7 +744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -765,7 +765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -787,7 +787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -808,7 +808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -826,7 +826,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -855,7 +855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -914,7 +914,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -929,7 +929,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
@@ -943,7 +943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
@@ -958,7 +958,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -972,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>38</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1229,8 +1229,11 @@
       <c r="D35" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>48</v>
       </c>
@@ -1245,7 +1248,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1296,7 +1299,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1325,7 +1328,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1340,7 +1343,7 @@
       </c>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -1368,7 +1371,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>37</v>
       </c>
@@ -1383,7 +1386,7 @@
       </c>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Finit A17: Ajout jingle sound
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810E04A9-B1A0-4507-A3D9-9F47F572D377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC083BF-2230-47E1-9044-7E8AD042406C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -667,11 +667,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.81640625" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
@@ -1155,6 +1155,9 @@
       <c r="D29" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
@@ -1267,7 +1270,9 @@
       <c r="D36" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="10"/>
+      <c r="E36" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">

</xml_diff>

<commit_message>
Fait la tâche A4
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC083BF-2230-47E1-9044-7E8AD042406C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E494E02-6826-46F9-AAA8-B9D2FBF15C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -668,10 +668,10 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.81640625" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
@@ -1403,6 +1403,9 @@
       </c>
       <c r="D44" t="s">
         <v>53</v>
+      </c>
+      <c r="E44" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ajouter vector2 pour jimmy
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E494E02-6826-46F9-AAA8-B9D2FBF15C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE594F0B-4989-405F-9102-F59AB22446B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -667,17 +667,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.81640625" style="1"/>
+    <col min="1" max="3" width="8.77734375" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +694,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -722,7 +722,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -744,7 +744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -765,7 +765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -787,7 +787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -808,7 +808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -826,7 +826,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -855,7 +855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -917,7 +917,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -934,7 +934,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
@@ -951,7 +951,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
@@ -968,7 +968,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -985,7 +985,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1078,8 +1078,11 @@
       <c r="D24" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -1092,8 +1095,11 @@
       <c r="D25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1110,7 +1116,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -1125,7 +1131,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1176,7 +1182,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1191,7 +1197,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1212,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>38</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1257,7 +1263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>48</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1291,7 +1297,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1308,7 +1314,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1325,7 +1331,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1357,7 +1363,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -1408,7 +1414,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>37</v>
       </c>
@@ -1423,7 +1429,7 @@
       </c>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1440,7 +1446,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
remove duplicate Taxi code from JAD
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE594F0B-4989-405F-9102-F59AB22446B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD23F9BF-5590-4272-B661-5468C87A6D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -667,17 +667,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="8.77734375" style="1"/>
+    <col min="1" max="3" width="8.81640625" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +694,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -722,7 +722,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -744,7 +744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -765,7 +765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -787,7 +787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -808,7 +808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -826,7 +826,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
@@ -841,7 +841,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -855,7 +855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
@@ -870,7 +870,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -917,7 +917,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -934,7 +934,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
@@ -951,7 +951,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
@@ -968,7 +968,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -985,7 +985,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
@@ -1210,9 +1210,11 @@
       <c r="D32" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E32" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -1229,7 +1231,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>38</v>
       </c>
@@ -1246,7 +1248,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1263,7 +1265,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>48</v>
       </c>
@@ -1280,7 +1282,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1297,7 +1299,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1316,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1331,7 +1333,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>17</v>
       </c>
@@ -1348,7 +1350,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1363,7 +1365,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1380,7 +1382,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
@@ -1397,7 +1399,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -1414,7 +1416,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>37</v>
       </c>
@@ -1429,7 +1431,7 @@
       </c>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -1446,7 +1448,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
fait la tâche M3
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcs\Documents\Projects\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD23F9BF-5590-4272-B661-5468C87A6D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39706FA8-980F-4525-A977-DAF7D088A3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -668,10 +668,10 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.81640625" style="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
@@ -1363,7 +1363,9 @@
       <c r="D41" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
@@ -1429,7 +1431,9 @@
       <c r="D45" t="s">
         <v>53</v>
       </c>
-      <c r="E45" s="10"/>
+      <c r="E45" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">

</xml_diff>

<commit_message>
Fin des taches avec le gamepad fonctionnel.
</commit_message>
<xml_diff>
--- a/420-5GP-BB-TP2-Repartition_des_taches.xlsx
+++ b/420-5GP-BB-TP2-Repartition_des_taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\TP2-Maintenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaldi\Desktop\TP2-Maintenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD23F9BF-5590-4272-B661-5468C87A6D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F95857B-E4A1-4165-A854-82C7BA8512F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{7E336F36-C994-417A-AD3F-7EC1A752D20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="56">
   <si>
     <t>Code</t>
   </si>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07939810-A45D-4268-84BC-8B7EA99A1C9A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -707,6 +707,9 @@
       <c r="D2" t="s">
         <v>52</v>
       </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -721,6 +724,9 @@
       <c r="D3" t="s">
         <v>52</v>
       </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
@@ -735,7 +741,9 @@
       <c r="D4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" t="s">
         <v>52</v>
       </c>
@@ -757,6 +765,9 @@
       <c r="D5" t="s">
         <v>52</v>
       </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
       <c r="I5" t="s">
         <v>51</v>
       </c>
@@ -778,7 +789,9 @@
       <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
       <c r="I6" t="s">
         <v>54</v>
       </c>
@@ -800,6 +813,9 @@
       <c r="D7" t="s">
         <v>52</v>
       </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
       <c r="I7" t="s">
         <v>53</v>
       </c>
@@ -821,6 +837,9 @@
       <c r="D8" t="s">
         <v>52</v>
       </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
       <c r="J8">
         <f>SUM(J4:J7)</f>
         <v>153</v>
@@ -839,7 +858,9 @@
       <c r="D9" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
@@ -854,6 +875,9 @@
       <c r="D10" t="s">
         <v>52</v>
       </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
@@ -868,7 +892,9 @@
       <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -883,7 +909,9 @@
       <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
@@ -898,7 +926,9 @@
       <c r="D13" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
@@ -998,7 +1028,7 @@
       <c r="D19" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1015,6 +1045,9 @@
       <c r="D20" t="s">
         <v>51</v>
       </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
@@ -1046,7 +1079,9 @@
       <c r="D22" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="10"/>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
@@ -1195,7 +1230,9 @@
       <c r="D31" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
@@ -1363,7 +1400,9 @@
       <c r="D41" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
@@ -1429,7 +1468,9 @@
       <c r="D45" t="s">
         <v>53</v>
       </c>
-      <c r="E45" s="10"/>
+      <c r="E45" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">

</xml_diff>